<commit_message>
code cleaning and debugging
Bug in paramsoptimisation.m and calcLikelihood.m
</commit_message>
<xml_diff>
--- a/code/ONET/task_data.xlsx
+++ b/code/ONET/task_data.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$331</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>occ1990dd</t>
   </si>
@@ -35,15 +38,12 @@
   <si>
     <t>Training label</t>
   </si>
-  <si>
-    <t/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,8 +53,23 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -75,14 +90,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,10 +435,13 @@
   <dimension ref="A1:F331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
@@ -491,9 +514,7 @@
       <c r="E4">
         <v>0.24182163178900001</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
@@ -529,9 +550,7 @@
       <c r="E6">
         <v>0.180020093918</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
@@ -585,9 +604,7 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
@@ -699,9 +716,7 @@
       <c r="E15">
         <v>0.23659157753000001</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
@@ -809,9 +824,7 @@
       <c r="E21">
         <v>1.2762511968600001</v>
       </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
@@ -847,9 +860,7 @@
       <c r="E23">
         <v>9.8537154495699997E-2</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
@@ -977,9 +988,7 @@
       <c r="E30">
         <v>0.99135619401899999</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
@@ -1087,9 +1096,7 @@
       <c r="E36">
         <v>0.220259174705</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
@@ -1107,9 +1114,7 @@
       <c r="E37">
         <v>0.24026155471800001</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
@@ -1127,9 +1132,7 @@
       <c r="E38">
         <v>0.35686612129200002</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
@@ -1165,9 +1168,7 @@
       <c r="E40">
         <v>2.0132176876100001</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
@@ -1203,9 +1204,7 @@
       <c r="E42">
         <v>1.0447717905</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
@@ -1223,9 +1222,7 @@
       <c r="E43">
         <v>0.94451928138700003</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
@@ -1243,9 +1240,7 @@
       <c r="E44">
         <v>2.9114632606500002</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
@@ -1263,9 +1258,7 @@
       <c r="E45">
         <v>1.0412728786500001</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
@@ -1283,8 +1276,8 @@
       <c r="E46">
         <v>1.75593221188</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>5</v>
+      <c r="F46" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1303,9 +1296,7 @@
       <c r="E47">
         <v>2.3291063308700002</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
@@ -1395,8 +1386,8 @@
       <c r="E52">
         <v>2.3904728889500002</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>5</v>
+      <c r="F52" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1559,9 +1550,7 @@
       <c r="E61">
         <v>0.267298966646</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
@@ -1579,9 +1568,7 @@
       <c r="E62">
         <v>2.6327002048499999</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
@@ -1599,9 +1586,7 @@
       <c r="E63">
         <v>2.2833597660099998</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6">
       <c r="A64">
@@ -1619,9 +1604,7 @@
       <c r="E64">
         <v>0.75784087181100002</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6">
       <c r="A65">
@@ -1639,9 +1622,7 @@
       <c r="E65">
         <v>1.70457601547</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6">
       <c r="A66">
@@ -1677,9 +1658,7 @@
       <c r="E67">
         <v>0.17544047534500001</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6">
       <c r="A68">
@@ -1715,9 +1694,7 @@
       <c r="E69">
         <v>1.92669272423</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6">
       <c r="A70">
@@ -1735,9 +1712,7 @@
       <c r="E70">
         <v>0.18317864835299999</v>
       </c>
-      <c r="F70" s="1">
-        <v>0</v>
-      </c>
+      <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6">
       <c r="A71">
@@ -1755,9 +1730,7 @@
       <c r="E71">
         <v>8.1264972686799997E-2</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6">
       <c r="A72">
@@ -1775,9 +1748,7 @@
       <c r="E72">
         <v>0.99627357721300003</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6">
       <c r="A73">
@@ -1813,9 +1784,7 @@
       <c r="E74">
         <v>9.6428237855400001E-2</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6">
       <c r="A75">
@@ -1833,9 +1802,7 @@
       <c r="E75">
         <v>7.7916666865299994E-2</v>
       </c>
-      <c r="F75" s="1">
-        <v>0</v>
-      </c>
+      <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6">
       <c r="A76">
@@ -1853,9 +1820,7 @@
       <c r="E76">
         <v>0.87748110294299997</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6">
       <c r="A77">
@@ -1873,9 +1838,7 @@
       <c r="E77">
         <v>2.50366632827E-3</v>
       </c>
-      <c r="F77" s="1">
-        <v>0</v>
-      </c>
+      <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78">
@@ -1931,9 +1894,7 @@
       <c r="E80">
         <v>0.47031089663499998</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
@@ -1951,9 +1912,7 @@
       <c r="E81">
         <v>3.8321542739900001</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
@@ -1989,9 +1948,7 @@
       <c r="E83">
         <v>0.19506081938700001</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
@@ -2027,9 +1984,7 @@
       <c r="E85">
         <v>10</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
@@ -2047,9 +2002,7 @@
       <c r="E86">
         <v>1.02520310879</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
@@ -2085,9 +2038,7 @@
       <c r="E88">
         <v>0</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
@@ -2105,9 +2056,7 @@
       <c r="E89">
         <v>5.84612798691</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
@@ -2125,9 +2074,7 @@
       <c r="E90">
         <v>0.51678180694599996</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
@@ -2181,9 +2128,7 @@
       <c r="E93">
         <v>2.43902206421</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6">
       <c r="A94">
@@ -2237,9 +2182,7 @@
       <c r="E96">
         <v>1.1950006485</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
@@ -2257,9 +2200,7 @@
       <c r="E97">
         <v>0.123172998428</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
@@ -2349,9 +2290,7 @@
       <c r="E102">
         <v>5.0220112800600001</v>
       </c>
-      <c r="F102" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
@@ -2369,9 +2308,7 @@
       <c r="E103">
         <v>0</v>
       </c>
-      <c r="F103" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
@@ -2389,9 +2326,7 @@
       <c r="E104">
         <v>0.42961564660099999</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
@@ -2427,9 +2362,7 @@
       <c r="E106">
         <v>0.46539068222000002</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F106" s="1"/>
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
@@ -2447,9 +2380,7 @@
       <c r="E107">
         <v>0.15840238332699999</v>
       </c>
-      <c r="F107" s="1">
-        <v>1</v>
-      </c>
+      <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6">
       <c r="A108">
@@ -2665,9 +2596,7 @@
       <c r="E119">
         <v>0.69608092308000002</v>
       </c>
-      <c r="F119" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6">
       <c r="A120">
@@ -2721,9 +2650,7 @@
       <c r="E122">
         <v>1.4969248324600001E-2</v>
       </c>
-      <c r="F122" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F122" s="1"/>
     </row>
     <row r="123" spans="1:6">
       <c r="A123">
@@ -3015,9 +2942,7 @@
       <c r="E138">
         <v>3.4031324088599997E-2</v>
       </c>
-      <c r="F138" s="1">
-        <v>1</v>
-      </c>
+      <c r="F138" s="1"/>
     </row>
     <row r="139" spans="1:6">
       <c r="A139">
@@ -3035,9 +2960,7 @@
       <c r="E139">
         <v>0</v>
       </c>
-      <c r="F139" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F139" s="1"/>
     </row>
     <row r="140" spans="1:6">
       <c r="A140">
@@ -3129,9 +3052,7 @@
       <c r="E144">
         <v>4.3640844523899998E-2</v>
       </c>
-      <c r="F144" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F144" s="1"/>
     </row>
     <row r="145" spans="1:6">
       <c r="A145">
@@ -3223,9 +3144,7 @@
       <c r="E149">
         <v>0.17804564535600001</v>
       </c>
-      <c r="F149" s="1">
-        <v>0</v>
-      </c>
+      <c r="F149" s="1"/>
     </row>
     <row r="150" spans="1:6">
       <c r="A150">
@@ -3481,9 +3400,7 @@
       <c r="E163">
         <v>0.36321029066999999</v>
       </c>
-      <c r="F163" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F163" s="1"/>
     </row>
     <row r="164" spans="1:6">
       <c r="A164">
@@ -3665,9 +3582,7 @@
       <c r="E173">
         <v>9.2692367732500003E-2</v>
       </c>
-      <c r="F173" s="1">
-        <v>0</v>
-      </c>
+      <c r="F173" s="1"/>
     </row>
     <row r="174" spans="1:6">
       <c r="A174">
@@ -3703,9 +3618,7 @@
       <c r="E175">
         <v>1.6133992671999999</v>
       </c>
-      <c r="F175" s="1">
-        <v>1</v>
-      </c>
+      <c r="F175" s="1"/>
     </row>
     <row r="176" spans="1:6">
       <c r="A176">
@@ -3795,9 +3708,7 @@
       <c r="E180">
         <v>2.7295017242399999</v>
       </c>
-      <c r="F180" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F180" s="1"/>
     </row>
     <row r="181" spans="1:6">
       <c r="A181">
@@ -3869,9 +3780,7 @@
       <c r="E184">
         <v>0.10640769451900001</v>
       </c>
-      <c r="F184" s="1">
-        <v>0</v>
-      </c>
+      <c r="F184" s="1"/>
     </row>
     <row r="185" spans="1:6">
       <c r="A185">
@@ -3889,9 +3798,7 @@
       <c r="E185">
         <v>1.77721488476</v>
       </c>
-      <c r="F185" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F185" s="1"/>
     </row>
     <row r="186" spans="1:6">
       <c r="A186">
@@ -3909,9 +3816,7 @@
       <c r="E186">
         <v>1.09161019325</v>
       </c>
-      <c r="F186" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F186" s="1"/>
     </row>
     <row r="187" spans="1:6">
       <c r="A187">
@@ -3947,9 +3852,7 @@
       <c r="E188">
         <v>2.1467530727400002</v>
       </c>
-      <c r="F188" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F188" s="1"/>
     </row>
     <row r="189" spans="1:6">
       <c r="A189">
@@ -3967,9 +3870,7 @@
       <c r="E189">
         <v>1.8413126468700001</v>
       </c>
-      <c r="F189" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F189" s="1"/>
     </row>
     <row r="190" spans="1:6">
       <c r="A190">
@@ -4023,9 +3924,7 @@
       <c r="E192">
         <v>0.99337637424500003</v>
       </c>
-      <c r="F192" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F192" s="1"/>
     </row>
     <row r="193" spans="1:6">
       <c r="A193">
@@ -4097,9 +3996,7 @@
       <c r="E196">
         <v>2.4206709861800002</v>
       </c>
-      <c r="F196" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F196" s="1"/>
     </row>
     <row r="197" spans="1:6">
       <c r="A197">
@@ -4135,9 +4032,7 @@
       <c r="E198">
         <v>2.2883684635199999</v>
       </c>
-      <c r="F198" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F198" s="1"/>
     </row>
     <row r="199" spans="1:6">
       <c r="A199">
@@ -4299,9 +4194,7 @@
       <c r="E207">
         <v>0.92298388481100002</v>
       </c>
-      <c r="F207" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F207" s="1"/>
     </row>
     <row r="208" spans="1:6">
       <c r="A208">
@@ -4337,9 +4230,7 @@
       <c r="E209">
         <v>2.1308827400200001</v>
       </c>
-      <c r="F209" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F209" s="1"/>
     </row>
     <row r="210" spans="1:6">
       <c r="A210">
@@ -4537,9 +4428,7 @@
       <c r="E220">
         <v>1.0882999897000001</v>
       </c>
-      <c r="F220" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F220" s="1"/>
     </row>
     <row r="221" spans="1:6">
       <c r="A221">
@@ -4629,9 +4518,7 @@
       <c r="E225">
         <v>2.7479462623600002</v>
       </c>
-      <c r="F225" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F225" s="1"/>
     </row>
     <row r="226" spans="1:6">
       <c r="A226">
@@ -4667,9 +4554,7 @@
       <c r="E227">
         <v>2.72767901421</v>
       </c>
-      <c r="F227" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F227" s="1"/>
     </row>
     <row r="228" spans="1:6">
       <c r="A228">
@@ -4777,9 +4662,7 @@
       <c r="E233">
         <v>2.5487990379299998</v>
       </c>
-      <c r="F233" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F233" s="1"/>
     </row>
     <row r="234" spans="1:6">
       <c r="A234">
@@ -4797,9 +4680,7 @@
       <c r="E234">
         <v>2.6185131073000001</v>
       </c>
-      <c r="F234" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F234" s="1"/>
     </row>
     <row r="235" spans="1:6">
       <c r="A235">
@@ -4943,9 +4824,7 @@
       <c r="E242">
         <v>2.9181141853299999</v>
       </c>
-      <c r="F242" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F242" s="1"/>
     </row>
     <row r="243" spans="1:6">
       <c r="A243">
@@ -4981,9 +4860,7 @@
       <c r="E244">
         <v>2.3627536296799998</v>
       </c>
-      <c r="F244" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F244" s="1"/>
     </row>
     <row r="245" spans="1:6">
       <c r="A245">
@@ -5109,9 +4986,7 @@
       <c r="E251">
         <v>5.4813090711800003E-2</v>
       </c>
-      <c r="F251" t="s">
-        <v>5</v>
-      </c>
+      <c r="F251" s="1"/>
     </row>
     <row r="252" spans="1:6">
       <c r="A252">
@@ -5147,9 +5022,7 @@
       <c r="E253">
         <v>2.3239741325400001</v>
       </c>
-      <c r="F253">
-        <v>1</v>
-      </c>
+      <c r="F253" s="1"/>
     </row>
     <row r="254" spans="1:6">
       <c r="A254">
@@ -5203,9 +5076,7 @@
       <c r="E256">
         <v>2.04091310501</v>
       </c>
-      <c r="F256" t="s">
-        <v>5</v>
-      </c>
+      <c r="F256" s="1"/>
     </row>
     <row r="257" spans="1:6">
       <c r="A257">
@@ -5295,9 +5166,7 @@
       <c r="E261">
         <v>1.78905010223</v>
       </c>
-      <c r="F261" t="s">
-        <v>5</v>
-      </c>
+      <c r="F261" s="1"/>
     </row>
     <row r="262" spans="1:6">
       <c r="A262">
@@ -5315,9 +5184,7 @@
       <c r="E262">
         <v>1.8278396129600001</v>
       </c>
-      <c r="F262" t="s">
-        <v>5</v>
-      </c>
+      <c r="F262" s="1"/>
     </row>
     <row r="263" spans="1:6">
       <c r="A263">
@@ -5335,9 +5202,7 @@
       <c r="E263">
         <v>0.41132521629300001</v>
       </c>
-      <c r="F263" t="s">
-        <v>5</v>
-      </c>
+      <c r="F263" s="1"/>
     </row>
     <row r="264" spans="1:6">
       <c r="A264">
@@ -5355,9 +5220,7 @@
       <c r="E264">
         <v>0</v>
       </c>
-      <c r="F264" t="s">
-        <v>5</v>
-      </c>
+      <c r="F264" s="1"/>
     </row>
     <row r="265" spans="1:6">
       <c r="A265">
@@ -5429,9 +5292,7 @@
       <c r="E268">
         <v>1.73963141441</v>
       </c>
-      <c r="F268" t="s">
-        <v>5</v>
-      </c>
+      <c r="F268" s="1"/>
     </row>
     <row r="269" spans="1:6">
       <c r="A269">
@@ -5467,9 +5328,7 @@
       <c r="E270">
         <v>1.8666840791699999</v>
       </c>
-      <c r="F270" t="s">
-        <v>5</v>
-      </c>
+      <c r="F270" s="1"/>
     </row>
     <row r="271" spans="1:6">
       <c r="A271">
@@ -5595,9 +5454,7 @@
       <c r="E277">
         <v>0.89073300361600005</v>
       </c>
-      <c r="F277" t="s">
-        <v>5</v>
-      </c>
+      <c r="F277" s="1"/>
     </row>
     <row r="278" spans="1:6">
       <c r="A278">
@@ -5687,9 +5544,7 @@
       <c r="E282">
         <v>1.02786231041</v>
       </c>
-      <c r="F282" t="s">
-        <v>5</v>
-      </c>
+      <c r="F282" s="1"/>
     </row>
     <row r="283" spans="1:6">
       <c r="A283">
@@ -5797,7 +5652,7 @@
       <c r="E288">
         <v>3.2864172458600001</v>
       </c>
-      <c r="F288">
+      <c r="F288" s="1">
         <v>1</v>
       </c>
     </row>
@@ -5853,9 +5708,7 @@
       <c r="E291">
         <v>0.79978913068799995</v>
       </c>
-      <c r="F291" t="s">
-        <v>5</v>
-      </c>
+      <c r="F291" s="1"/>
     </row>
     <row r="292" spans="1:6">
       <c r="A292">
@@ -5927,9 +5780,7 @@
       <c r="E295">
         <v>0.59447997808499997</v>
       </c>
-      <c r="F295" t="s">
-        <v>5</v>
-      </c>
+      <c r="F295" s="1"/>
     </row>
     <row r="296" spans="1:6">
       <c r="A296">
@@ -5947,9 +5798,7 @@
       <c r="E296">
         <v>1.1415371894799999</v>
       </c>
-      <c r="F296" t="s">
-        <v>5</v>
-      </c>
+      <c r="F296" s="1"/>
     </row>
     <row r="297" spans="1:6">
       <c r="A297">
@@ -6057,9 +5906,7 @@
       <c r="E302">
         <v>0.348211586475</v>
       </c>
-      <c r="F302" t="s">
-        <v>5</v>
-      </c>
+      <c r="F302" s="1"/>
     </row>
     <row r="303" spans="1:6">
       <c r="A303">
@@ -6095,9 +5942,7 @@
       <c r="E304">
         <v>0.643265962601</v>
       </c>
-      <c r="F304" t="s">
-        <v>5</v>
-      </c>
+      <c r="F304" s="1"/>
     </row>
     <row r="305" spans="1:6">
       <c r="A305">
@@ -6133,9 +5978,7 @@
       <c r="E306">
         <v>3.06212329865</v>
       </c>
-      <c r="F306" t="s">
-        <v>5</v>
-      </c>
+      <c r="F306" s="1"/>
     </row>
     <row r="307" spans="1:6">
       <c r="A307">
@@ -6171,9 +6014,7 @@
       <c r="E308">
         <v>0.85642039775800005</v>
       </c>
-      <c r="F308" t="s">
-        <v>5</v>
-      </c>
+      <c r="F308" s="1"/>
     </row>
     <row r="309" spans="1:6">
       <c r="A309">
@@ -6191,9 +6032,7 @@
       <c r="E309">
         <v>4.6560578346300003</v>
       </c>
-      <c r="F309">
-        <v>1</v>
-      </c>
+      <c r="F309" s="1"/>
     </row>
     <row r="310" spans="1:6">
       <c r="A310">
@@ -6211,9 +6050,7 @@
       <c r="E310">
         <v>4.9500937461900003</v>
       </c>
-      <c r="F310" t="s">
-        <v>5</v>
-      </c>
+      <c r="F310" s="1"/>
     </row>
     <row r="311" spans="1:6">
       <c r="A311">
@@ -6231,7 +6068,7 @@
       <c r="E311">
         <v>4.8360834121699998</v>
       </c>
-      <c r="F311">
+      <c r="F311" s="1">
         <v>1</v>
       </c>
     </row>
@@ -6251,7 +6088,7 @@
       <c r="E312">
         <v>5</v>
       </c>
-      <c r="F312">
+      <c r="F312" s="1">
         <v>1</v>
       </c>
     </row>
@@ -6397,9 +6234,7 @@
       <c r="E320">
         <v>4.7782859802199997</v>
       </c>
-      <c r="F320" t="s">
-        <v>5</v>
-      </c>
+      <c r="F320" s="1"/>
     </row>
     <row r="321" spans="1:6">
       <c r="A321">
@@ -6417,9 +6252,7 @@
       <c r="E321">
         <v>2.2113845348400001</v>
       </c>
-      <c r="F321" t="s">
-        <v>5</v>
-      </c>
+      <c r="F321" s="1"/>
     </row>
     <row r="322" spans="1:6">
       <c r="A322">
@@ -6455,9 +6288,7 @@
       <c r="E323">
         <v>2.5141761302900001</v>
       </c>
-      <c r="F323" t="s">
-        <v>5</v>
-      </c>
+      <c r="F323" s="1"/>
     </row>
     <row r="324" spans="1:6">
       <c r="A324">
@@ -6605,6 +6436,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>